<commit_message>
Ashok kumar Time sheet
</commit_message>
<xml_diff>
--- a/Ashok/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
+++ b/Ashok/Timesheet/Schwall_TraineeName_Timesheet_June_2021.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="1" r:id="rId1"/>
     <sheet name="Week2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>SlNo</t>
   </si>
@@ -39,11 +39,26 @@
   <si>
     <t>SCHWALL WEEKLY TIMESHEET</t>
   </si>
+  <si>
+    <t>04.06.2021</t>
+  </si>
+  <si>
+    <t>05.06.2021</t>
+  </si>
+  <si>
+    <t>06.06.2021</t>
+  </si>
+  <si>
+    <t>Arraylist</t>
+  </si>
+  <si>
+    <t>Insert,Search,print,remove operation for Student details</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -539,19 +554,19 @@
   <dimension ref="B1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="44.90625" customWidth="1"/>
-    <col min="6" max="6" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
@@ -560,7 +575,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -577,994 +592,1012 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="2"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="2"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="2"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="2"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="2"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="2"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="2"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="2"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="2"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="2"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="2"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="2"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="2"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="2"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="2"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="2"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="2"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="2"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="2"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="2"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="2"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="2"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="2"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="2"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115" s="2"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B116" s="2"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117" s="2"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B118" s="2"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B119" s="2"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B120" s="2"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B121" s="2"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="2"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B123" s="2"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="2"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="3"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="2"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="2"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="3"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="2"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="2"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="2"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="3"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="2"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="2"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="3"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="2"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="2"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="2"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="2"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="2"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="2"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="3"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="2"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="2"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B145" s="4"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -1588,16 +1621,16 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="44.90625" customWidth="1"/>
-    <col min="6" max="6" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1639,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1623,994 +1656,994 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="2"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="2"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="2"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="2"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="2"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="2"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="2"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="2"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="2"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="2"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="2"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="2"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="2"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="2"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="2"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="2"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="2"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="2"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="2"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="2"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="2"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="2"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="2"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="2"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="2"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="2"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="2"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="2"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="2"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115" s="2"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B116" s="2"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117" s="2"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B118" s="2"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B119" s="2"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B120" s="2"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B121" s="2"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="2"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B123" s="2"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="2"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="3"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="2"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="2"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="3"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="2"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="2"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="2"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="3"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="2"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="2"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="3"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="2"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="2"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="2"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="2"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="2"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="2"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="3"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="2"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="2"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B145" s="4"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>

</xml_diff>